<commit_message>
Update Race by province and gender 2016.xlsx
</commit_message>
<xml_diff>
--- a/Resources/Race by province and gender 2016.xlsx
+++ b/Resources/Race by province and gender 2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haeze\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haeze\Documents\GitHub\Project2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6ACEAC2B-94B9-49AD-B8ED-4D95974598F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD7B879-822B-49F1-BB62-25D6417AEA71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Finished Sheet" sheetId="2" r:id="rId1"/>
@@ -208,19 +208,19 @@
     <t>Vietnamese</t>
   </si>
   <si>
-    <t>First Nations (North American Indian)</t>
-  </si>
-  <si>
     <t>Canadian</t>
   </si>
   <si>
     <t>Jamaican</t>
+  </si>
+  <si>
+    <t>First Nations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,11 +1063,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1209,12 +1209,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>200290</v>
@@ -1348,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>902315</v>
@@ -2822,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>17325</v>

</xml_diff>